<commit_message>
📊 Update UrbanGulal_Consolidated_2026-01-13.xlsx - 2026-01-13T10:38:46.657Z
</commit_message>
<xml_diff>
--- a/reports/UrbanGulal_Consolidated_2026-01-13.xlsx
+++ b/reports/UrbanGulal_Consolidated_2026-01-13.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -441,63 +441,63 @@
         <v>Feedback</v>
       </c>
     </row>
-    <row r="2" xml:space="preserve">
+    <row r="2">
       <c r="A2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" t="str">
-        <v>2026-01-13 10:20</v>
+        <v>2026-01-13 10:38</v>
       </c>
       <c r="C2" t="str">
         <v>Pooja</v>
       </c>
       <c r="D2" t="str">
+        <v>9096648553</v>
+      </c>
+      <c r="E2" t="str">
+        <v>A 1608, Pune 411045</v>
+      </c>
+      <c r="F2" t="str">
+        <v>Girl Haldi Kunku Set x1</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2" t="str">
+        <v>NEW</v>
+      </c>
+      <c r="I2" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J2" t="str">
+        <v/>
+      </c>
+      <c r="K2" t="str">
+        <v/>
+      </c>
+      <c r="L2" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="3" xml:space="preserve">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="str">
+        <v>2026-01-13 10:20</v>
+      </c>
+      <c r="C3" t="str">
+        <v>Pooja</v>
+      </c>
+      <c r="D3" t="str">
         <v>02030443000</v>
       </c>
-      <c r="E2" t="str" xml:space="preserve">
+      <c r="E3" t="str" xml:space="preserve">
         <v xml:space="preserve">Level 1, Tower S3, CyberCity,
 Magarpatta City, Hadapsar, PUNE 411013</v>
       </c>
-      <c r="F2" t="str">
+      <c r="F3" t="str">
         <v>Girl Holding Hands Thali x1</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2" t="str">
-        <v>NEW</v>
-      </c>
-      <c r="I2" t="str">
-        <v>PENDING</v>
-      </c>
-      <c r="J2" t="str">
-        <v/>
-      </c>
-      <c r="K2" t="str">
-        <v/>
-      </c>
-      <c r="L2" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="str">
-        <v>2026-01-13 09:36</v>
-      </c>
-      <c r="C3" t="str">
-        <v>Pooja</v>
-      </c>
-      <c r="D3" t="str">
-        <v>9096648553</v>
-      </c>
-      <c r="E3" t="str">
-        <v>A 1608, Pune 411045</v>
-      </c>
-      <c r="F3" t="str">
-        <v>Girl Haldi Kunku Set x10</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -515,12 +515,50 @@
         <v/>
       </c>
       <c r="L3" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="str">
+        <v>2026-01-13 09:36</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Pooja</v>
+      </c>
+      <c r="D4" t="str">
+        <v>9096648553</v>
+      </c>
+      <c r="E4" t="str">
+        <v>A 1608, Pune 411045</v>
+      </c>
+      <c r="F4" t="str">
+        <v>Girl Haldi Kunku Set x10</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4" t="str">
+        <v>NEW</v>
+      </c>
+      <c r="I4" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J4" t="str">
+        <v/>
+      </c>
+      <c r="K4" t="str">
+        <v/>
+      </c>
+      <c r="L4" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L4"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -560,7 +598,7 @@
         <v>2026-01-13</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2">
         <v>0</v>

</xml_diff>

<commit_message>
📊 Update UrbanGulal_Consolidated_2026-01-13.xlsx - 2026-01-13T10:51:27.311Z
</commit_message>
<xml_diff>
--- a/reports/UrbanGulal_Consolidated_2026-01-13.xlsx
+++ b/reports/UrbanGulal_Consolidated_2026-01-13.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -443,22 +443,22 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" t="str">
-        <v>2026-01-13 10:38</v>
+        <v>2026-01-13 10:51</v>
       </c>
       <c r="C2" t="str">
-        <v>Pooja</v>
+        <v>Ajay Dwarkunde</v>
       </c>
       <c r="D2" t="str">
-        <v>9096648553</v>
+        <v>8087172173</v>
       </c>
       <c r="E2" t="str">
-        <v>A 1608, Pune 411045</v>
+        <v>wakad, pune 411057</v>
       </c>
       <c r="F2" t="str">
-        <v>Girl Haldi Kunku Set x1</v>
+        <v>Girl Holding Hands Thali x1, Kalash Haldi Kunku (Golden) x1, Kite Haldi Kunku Set x1</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -479,63 +479,63 @@
         <v/>
       </c>
     </row>
-    <row r="3" xml:space="preserve">
+    <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" t="str">
-        <v>2026-01-13 10:20</v>
+        <v>2026-01-13 10:38</v>
       </c>
       <c r="C3" t="str">
         <v>Pooja</v>
       </c>
       <c r="D3" t="str">
+        <v>9096648553</v>
+      </c>
+      <c r="E3" t="str">
+        <v>A 1608, Pune 411045</v>
+      </c>
+      <c r="F3" t="str">
+        <v>Girl Haldi Kunku Set x1</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3" t="str">
+        <v>NEW</v>
+      </c>
+      <c r="I3" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J3" t="str">
+        <v/>
+      </c>
+      <c r="K3" t="str">
+        <v/>
+      </c>
+      <c r="L3" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="4" xml:space="preserve">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="str">
+        <v>2026-01-13 10:20</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Pooja</v>
+      </c>
+      <c r="D4" t="str">
         <v>02030443000</v>
       </c>
-      <c r="E3" t="str" xml:space="preserve">
+      <c r="E4" t="str" xml:space="preserve">
         <v xml:space="preserve">Level 1, Tower S3, CyberCity,
 Magarpatta City, Hadapsar, PUNE 411013</v>
       </c>
-      <c r="F3" t="str">
+      <c r="F4" t="str">
         <v>Girl Holding Hands Thali x1</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3" t="str">
-        <v>NEW</v>
-      </c>
-      <c r="I3" t="str">
-        <v>PENDING</v>
-      </c>
-      <c r="J3" t="str">
-        <v/>
-      </c>
-      <c r="K3" t="str">
-        <v/>
-      </c>
-      <c r="L3" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4" t="str">
-        <v>2026-01-13 09:36</v>
-      </c>
-      <c r="C4" t="str">
-        <v>Pooja</v>
-      </c>
-      <c r="D4" t="str">
-        <v>9096648553</v>
-      </c>
-      <c r="E4" t="str">
-        <v>A 1608, Pune 411045</v>
-      </c>
-      <c r="F4" t="str">
-        <v>Girl Haldi Kunku Set x10</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -553,12 +553,50 @@
         <v/>
       </c>
       <c r="L4" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="str">
+        <v>2026-01-13 09:36</v>
+      </c>
+      <c r="C5" t="str">
+        <v>Pooja</v>
+      </c>
+      <c r="D5" t="str">
+        <v>9096648553</v>
+      </c>
+      <c r="E5" t="str">
+        <v>A 1608, Pune 411045</v>
+      </c>
+      <c r="F5" t="str">
+        <v>Girl Haldi Kunku Set x10</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5" t="str">
+        <v>NEW</v>
+      </c>
+      <c r="I5" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J5" t="str">
+        <v/>
+      </c>
+      <c r="K5" t="str">
+        <v/>
+      </c>
+      <c r="L5" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L5"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -598,7 +636,7 @@
         <v>2026-01-13</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2">
         <v>0</v>

</xml_diff>

<commit_message>
📊 Update UrbanGulal_Consolidated_2026-01-13.xlsx - 2026-01-13T16:40:32.087Z
</commit_message>
<xml_diff>
--- a/reports/UrbanGulal_Consolidated_2026-01-13.xlsx
+++ b/reports/UrbanGulal_Consolidated_2026-01-13.xlsx
@@ -464,7 +464,7 @@
         <v>0</v>
       </c>
       <c r="H2" t="str">
-        <v>NEW</v>
+        <v>CANCELLED</v>
       </c>
       <c r="I2" t="str">
         <v>PENDING</v>
@@ -473,7 +473,7 @@
         <v/>
       </c>
       <c r="K2" t="str">
-        <v/>
+        <v>test</v>
       </c>
       <c r="L2" t="str">
         <v/>
@@ -642,7 +642,7 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2">
         <v>0</v>

</xml_diff>

<commit_message>
📊 Update UrbanGulal_Consolidated_2026-01-13.xlsx - 2026-01-13T16:54:25.039Z
</commit_message>
<xml_diff>
--- a/reports/UrbanGulal_Consolidated_2026-01-13.xlsx
+++ b/reports/UrbanGulal_Consolidated_2026-01-13.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -441,30 +441,31 @@
         <v>Feedback</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" xml:space="preserve">
       <c r="A2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" t="str">
-        <v>2026-01-13 10:51</v>
+        <v>2026-01-13 16:54</v>
       </c>
       <c r="C2" t="str">
-        <v>Ajay Dwarkunde</v>
+        <v>Pooja</v>
       </c>
       <c r="D2" t="str">
-        <v>8087172173</v>
-      </c>
-      <c r="E2" t="str">
-        <v>wakad, pune 411057</v>
+        <v>9096648553</v>
+      </c>
+      <c r="E2" t="str" xml:space="preserve">
+        <v xml:space="preserve">Level 1, Tower S3, CyberCity,
+Magarpatta City, Hadapsar, PUNE 411013</v>
       </c>
       <c r="F2" t="str">
-        <v>Girl Holding Hands Thali x1, Kalash Haldi Kunku (Golden) x1, Kite Haldi Kunku Set x1</v>
+        <v>Girl Holding Hands Thali x1</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2" t="str">
-        <v>CANCELLED</v>
+        <v>NEW</v>
       </c>
       <c r="I2" t="str">
         <v>PENDING</v>
@@ -473,7 +474,7 @@
         <v/>
       </c>
       <c r="K2" t="str">
-        <v>test</v>
+        <v/>
       </c>
       <c r="L2" t="str">
         <v/>
@@ -481,28 +482,28 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" t="str">
-        <v>2026-01-13 10:38</v>
+        <v>2026-01-13 10:51</v>
       </c>
       <c r="C3" t="str">
-        <v>Pooja</v>
+        <v>Ajay Dwarkunde</v>
       </c>
       <c r="D3" t="str">
-        <v>9096648553</v>
+        <v>8087172173</v>
       </c>
       <c r="E3" t="str">
-        <v>A 1608, Pune 411045</v>
+        <v>wakad, pune 411057</v>
       </c>
       <c r="F3" t="str">
-        <v>Girl Haldi Kunku Set x1</v>
+        <v>Girl Holding Hands Thali x1, Kalash Haldi Kunku (Golden) x1, Kite Haldi Kunku Set x1</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="H3" t="str">
-        <v>NEW</v>
+        <v>CANCELLED</v>
       </c>
       <c r="I3" t="str">
         <v>PENDING</v>
@@ -511,69 +512,69 @@
         <v/>
       </c>
       <c r="K3" t="str">
-        <v/>
+        <v>test</v>
       </c>
       <c r="L3" t="str">
         <v/>
       </c>
     </row>
-    <row r="4" xml:space="preserve">
+    <row r="4">
       <c r="A4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="str">
-        <v>2026-01-13 10:20</v>
+        <v>2026-01-13 10:38</v>
       </c>
       <c r="C4" t="str">
         <v>Pooja</v>
       </c>
       <c r="D4" t="str">
+        <v>9096648553</v>
+      </c>
+      <c r="E4" t="str">
+        <v>A 1608, Pune 411045</v>
+      </c>
+      <c r="F4" t="str">
+        <v>Girl Haldi Kunku Set x1</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4" t="str">
+        <v>NEW</v>
+      </c>
+      <c r="I4" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J4" t="str">
+        <v/>
+      </c>
+      <c r="K4" t="str">
+        <v/>
+      </c>
+      <c r="L4" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="5" xml:space="preserve">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="str">
+        <v>2026-01-13 10:20</v>
+      </c>
+      <c r="C5" t="str">
+        <v>Pooja</v>
+      </c>
+      <c r="D5" t="str">
         <v>02030443000</v>
       </c>
-      <c r="E4" t="str" xml:space="preserve">
+      <c r="E5" t="str" xml:space="preserve">
         <v xml:space="preserve">Level 1, Tower S3, CyberCity,
 Magarpatta City, Hadapsar, PUNE 411013</v>
       </c>
-      <c r="F4" t="str">
+      <c r="F5" t="str">
         <v>Girl Holding Hands Thali x1</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4" t="str">
-        <v>NEW</v>
-      </c>
-      <c r="I4" t="str">
-        <v>PENDING</v>
-      </c>
-      <c r="J4" t="str">
-        <v/>
-      </c>
-      <c r="K4" t="str">
-        <v/>
-      </c>
-      <c r="L4" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5" t="str">
-        <v>2026-01-13 09:36</v>
-      </c>
-      <c r="C5" t="str">
-        <v>Pooja</v>
-      </c>
-      <c r="D5" t="str">
-        <v>9096648553</v>
-      </c>
-      <c r="E5" t="str">
-        <v>A 1608, Pune 411045</v>
-      </c>
-      <c r="F5" t="str">
-        <v>Girl Haldi Kunku Set x10</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -591,12 +592,50 @@
         <v/>
       </c>
       <c r="L5" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="str">
+        <v>2026-01-13 09:36</v>
+      </c>
+      <c r="C6" t="str">
+        <v>Pooja</v>
+      </c>
+      <c r="D6" t="str">
+        <v>9096648553</v>
+      </c>
+      <c r="E6" t="str">
+        <v>A 1608, Pune 411045</v>
+      </c>
+      <c r="F6" t="str">
+        <v>Girl Haldi Kunku Set x10</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6" t="str">
+        <v>NEW</v>
+      </c>
+      <c r="I6" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J6" t="str">
+        <v/>
+      </c>
+      <c r="K6" t="str">
+        <v/>
+      </c>
+      <c r="L6" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L6"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -636,7 +675,7 @@
         <v>2026-01-13</v>
       </c>
       <c r="B2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <v>0</v>

</xml_diff>

<commit_message>
📊 Update UrbanGulal_Consolidated_2026-01-13.xlsx - 2026-01-13T18:47:18.208Z
</commit_message>
<xml_diff>
--- a/reports/UrbanGulal_Consolidated_2026-01-13.xlsx
+++ b/reports/UrbanGulal_Consolidated_2026-01-13.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -441,69 +441,69 @@
         <v>Feedback</v>
       </c>
     </row>
-    <row r="2" xml:space="preserve">
+    <row r="2">
       <c r="A2">
+        <v>6</v>
+      </c>
+      <c r="B2" t="str">
+        <v>2026-01-13 18:47</v>
+      </c>
+      <c r="C2" t="str">
+        <v>Sagar Borse</v>
+      </c>
+      <c r="D2" t="str">
+        <v>7588930329</v>
+      </c>
+      <c r="E2" t="str">
+        <v>Test,</v>
+      </c>
+      <c r="F2" t="str">
+        <v>Girl Haldi Kunku Set x1</v>
+      </c>
+      <c r="G2">
+        <v>25</v>
+      </c>
+      <c r="H2" t="str">
+        <v>NEW</v>
+      </c>
+      <c r="I2" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J2" t="str">
+        <v/>
+      </c>
+      <c r="K2" t="str">
+        <v/>
+      </c>
+      <c r="L2" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="3" xml:space="preserve">
+      <c r="A3">
         <v>5</v>
       </c>
-      <c r="B2" t="str">
+      <c r="B3" t="str">
         <v>2026-01-13 16:54</v>
       </c>
-      <c r="C2" t="str">
+      <c r="C3" t="str">
         <v>Pooja</v>
       </c>
-      <c r="D2" t="str">
+      <c r="D3" t="str">
         <v>9096648553</v>
       </c>
-      <c r="E2" t="str" xml:space="preserve">
+      <c r="E3" t="str" xml:space="preserve">
         <v xml:space="preserve">Level 1, Tower S3, CyberCity,
 Magarpatta City, Hadapsar, PUNE 411013</v>
       </c>
-      <c r="F2" t="str">
+      <c r="F3" t="str">
         <v>Girl Holding Hands Thali x1</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2" t="str">
-        <v>NEW</v>
-      </c>
-      <c r="I2" t="str">
-        <v>PENDING</v>
-      </c>
-      <c r="J2" t="str">
-        <v/>
-      </c>
-      <c r="K2" t="str">
-        <v/>
-      </c>
-      <c r="L2" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3">
-        <v>4</v>
-      </c>
-      <c r="B3" t="str">
-        <v>2026-01-13 10:51</v>
-      </c>
-      <c r="C3" t="str">
-        <v>Ajay Dwarkunde</v>
-      </c>
-      <c r="D3" t="str">
-        <v>8087172173</v>
-      </c>
-      <c r="E3" t="str">
-        <v>wakad, pune 411057</v>
-      </c>
-      <c r="F3" t="str">
-        <v>Girl Holding Hands Thali x1, Kalash Haldi Kunku (Golden) x1, Kite Haldi Kunku Set x1</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="H3" t="str">
-        <v>CANCELLED</v>
+        <v>NEW</v>
       </c>
       <c r="I3" t="str">
         <v>PENDING</v>
@@ -512,7 +512,7 @@
         <v/>
       </c>
       <c r="K3" t="str">
-        <v>test</v>
+        <v/>
       </c>
       <c r="L3" t="str">
         <v/>
@@ -520,28 +520,28 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" t="str">
-        <v>2026-01-13 10:38</v>
+        <v>2026-01-13 10:51</v>
       </c>
       <c r="C4" t="str">
-        <v>Pooja</v>
+        <v>Ajay Dwarkunde</v>
       </c>
       <c r="D4" t="str">
-        <v>9096648553</v>
+        <v>8087172173</v>
       </c>
       <c r="E4" t="str">
-        <v>A 1608, Pune 411045</v>
+        <v>wakad, pune 411057</v>
       </c>
       <c r="F4" t="str">
-        <v>Girl Haldi Kunku Set x1</v>
+        <v>Girl Holding Hands Thali x1, Kalash Haldi Kunku (Golden) x1, Kite Haldi Kunku Set x1</v>
       </c>
       <c r="G4">
         <v>0</v>
       </c>
       <c r="H4" t="str">
-        <v>NEW</v>
+        <v>CANCELLED</v>
       </c>
       <c r="I4" t="str">
         <v>PENDING</v>
@@ -550,69 +550,69 @@
         <v/>
       </c>
       <c r="K4" t="str">
-        <v/>
+        <v>test</v>
       </c>
       <c r="L4" t="str">
         <v/>
       </c>
     </row>
-    <row r="5" xml:space="preserve">
+    <row r="5">
       <c r="A5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5" t="str">
-        <v>2026-01-13 10:20</v>
+        <v>2026-01-13 10:38</v>
       </c>
       <c r="C5" t="str">
         <v>Pooja</v>
       </c>
       <c r="D5" t="str">
+        <v>9096648553</v>
+      </c>
+      <c r="E5" t="str">
+        <v>A 1608, Pune 411045</v>
+      </c>
+      <c r="F5" t="str">
+        <v>Girl Haldi Kunku Set x1</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5" t="str">
+        <v>NEW</v>
+      </c>
+      <c r="I5" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J5" t="str">
+        <v/>
+      </c>
+      <c r="K5" t="str">
+        <v/>
+      </c>
+      <c r="L5" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="6" xml:space="preserve">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" t="str">
+        <v>2026-01-13 10:20</v>
+      </c>
+      <c r="C6" t="str">
+        <v>Pooja</v>
+      </c>
+      <c r="D6" t="str">
         <v>02030443000</v>
       </c>
-      <c r="E5" t="str" xml:space="preserve">
+      <c r="E6" t="str" xml:space="preserve">
         <v xml:space="preserve">Level 1, Tower S3, CyberCity,
 Magarpatta City, Hadapsar, PUNE 411013</v>
       </c>
-      <c r="F5" t="str">
+      <c r="F6" t="str">
         <v>Girl Holding Hands Thali x1</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5" t="str">
-        <v>NEW</v>
-      </c>
-      <c r="I5" t="str">
-        <v>PENDING</v>
-      </c>
-      <c r="J5" t="str">
-        <v/>
-      </c>
-      <c r="K5" t="str">
-        <v/>
-      </c>
-      <c r="L5" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6" t="str">
-        <v>2026-01-13 09:36</v>
-      </c>
-      <c r="C6" t="str">
-        <v>Pooja</v>
-      </c>
-      <c r="D6" t="str">
-        <v>9096648553</v>
-      </c>
-      <c r="E6" t="str">
-        <v>A 1608, Pune 411045</v>
-      </c>
-      <c r="F6" t="str">
-        <v>Girl Haldi Kunku Set x10</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -633,9 +633,47 @@
         <v/>
       </c>
     </row>
+    <row r="7">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="str">
+        <v>2026-01-13 09:36</v>
+      </c>
+      <c r="C7" t="str">
+        <v>Pooja</v>
+      </c>
+      <c r="D7" t="str">
+        <v>9096648553</v>
+      </c>
+      <c r="E7" t="str">
+        <v>A 1608, Pune 411045</v>
+      </c>
+      <c r="F7" t="str">
+        <v>Girl Haldi Kunku Set x10</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7" t="str">
+        <v>NEW</v>
+      </c>
+      <c r="I7" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J7" t="str">
+        <v/>
+      </c>
+      <c r="K7" t="str">
+        <v/>
+      </c>
+      <c r="L7" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L7"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -675,7 +713,7 @@
         <v>2026-01-13</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -684,13 +722,13 @@
         <v>1</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
📊 Update UrbanGulal_Consolidated_2026-01-13.xlsx - 2026-01-13T18:48:06.072Z
</commit_message>
<xml_diff>
--- a/reports/UrbanGulal_Consolidated_2026-01-13.xlsx
+++ b/reports/UrbanGulal_Consolidated_2026-01-13.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -443,10 +443,10 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" t="str">
-        <v>2026-01-13 18:47</v>
+        <v>2026-01-13 18:48</v>
       </c>
       <c r="C2" t="str">
         <v>Sagar Borse</v>
@@ -455,13 +455,13 @@
         <v>7588930329</v>
       </c>
       <c r="E2" t="str">
-        <v>Test,</v>
+        <v>Test2,</v>
       </c>
       <c r="F2" t="str">
-        <v>Girl Haldi Kunku Set x1</v>
+        <v>Kite Haldi Kunku Set x10</v>
       </c>
       <c r="G2">
-        <v>25</v>
+        <v>300</v>
       </c>
       <c r="H2" t="str">
         <v>NEW</v>
@@ -479,69 +479,69 @@
         <v/>
       </c>
     </row>
-    <row r="3" xml:space="preserve">
+    <row r="3">
       <c r="A3">
+        <v>6</v>
+      </c>
+      <c r="B3" t="str">
+        <v>2026-01-13 18:47</v>
+      </c>
+      <c r="C3" t="str">
+        <v>Sagar Borse</v>
+      </c>
+      <c r="D3" t="str">
+        <v>7588930329</v>
+      </c>
+      <c r="E3" t="str">
+        <v>Test,</v>
+      </c>
+      <c r="F3" t="str">
+        <v>Girl Haldi Kunku Set x1</v>
+      </c>
+      <c r="G3">
+        <v>25</v>
+      </c>
+      <c r="H3" t="str">
+        <v>NEW</v>
+      </c>
+      <c r="I3" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J3" t="str">
+        <v/>
+      </c>
+      <c r="K3" t="str">
+        <v/>
+      </c>
+      <c r="L3" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="4" xml:space="preserve">
+      <c r="A4">
         <v>5</v>
       </c>
-      <c r="B3" t="str">
+      <c r="B4" t="str">
         <v>2026-01-13 16:54</v>
       </c>
-      <c r="C3" t="str">
+      <c r="C4" t="str">
         <v>Pooja</v>
       </c>
-      <c r="D3" t="str">
+      <c r="D4" t="str">
         <v>9096648553</v>
       </c>
-      <c r="E3" t="str" xml:space="preserve">
+      <c r="E4" t="str" xml:space="preserve">
         <v xml:space="preserve">Level 1, Tower S3, CyberCity,
 Magarpatta City, Hadapsar, PUNE 411013</v>
       </c>
-      <c r="F3" t="str">
+      <c r="F4" t="str">
         <v>Girl Holding Hands Thali x1</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3" t="str">
-        <v>NEW</v>
-      </c>
-      <c r="I3" t="str">
-        <v>PENDING</v>
-      </c>
-      <c r="J3" t="str">
-        <v/>
-      </c>
-      <c r="K3" t="str">
-        <v/>
-      </c>
-      <c r="L3" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4">
-        <v>4</v>
-      </c>
-      <c r="B4" t="str">
-        <v>2026-01-13 10:51</v>
-      </c>
-      <c r="C4" t="str">
-        <v>Ajay Dwarkunde</v>
-      </c>
-      <c r="D4" t="str">
-        <v>8087172173</v>
-      </c>
-      <c r="E4" t="str">
-        <v>wakad, pune 411057</v>
-      </c>
-      <c r="F4" t="str">
-        <v>Girl Holding Hands Thali x1, Kalash Haldi Kunku (Golden) x1, Kite Haldi Kunku Set x1</v>
       </c>
       <c r="G4">
         <v>0</v>
       </c>
       <c r="H4" t="str">
-        <v>CANCELLED</v>
+        <v>NEW</v>
       </c>
       <c r="I4" t="str">
         <v>PENDING</v>
@@ -550,7 +550,7 @@
         <v/>
       </c>
       <c r="K4" t="str">
-        <v>test</v>
+        <v/>
       </c>
       <c r="L4" t="str">
         <v/>
@@ -558,28 +558,28 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="str">
-        <v>2026-01-13 10:38</v>
+        <v>2026-01-13 10:51</v>
       </c>
       <c r="C5" t="str">
-        <v>Pooja</v>
+        <v>Ajay Dwarkunde</v>
       </c>
       <c r="D5" t="str">
-        <v>9096648553</v>
+        <v>8087172173</v>
       </c>
       <c r="E5" t="str">
-        <v>A 1608, Pune 411045</v>
+        <v>wakad, pune 411057</v>
       </c>
       <c r="F5" t="str">
-        <v>Girl Haldi Kunku Set x1</v>
+        <v>Girl Holding Hands Thali x1, Kalash Haldi Kunku (Golden) x1, Kite Haldi Kunku Set x1</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
       <c r="H5" t="str">
-        <v>NEW</v>
+        <v>CANCELLED</v>
       </c>
       <c r="I5" t="str">
         <v>PENDING</v>
@@ -588,69 +588,69 @@
         <v/>
       </c>
       <c r="K5" t="str">
-        <v/>
+        <v>test</v>
       </c>
       <c r="L5" t="str">
         <v/>
       </c>
     </row>
-    <row r="6" xml:space="preserve">
+    <row r="6">
       <c r="A6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B6" t="str">
-        <v>2026-01-13 10:20</v>
+        <v>2026-01-13 10:38</v>
       </c>
       <c r="C6" t="str">
         <v>Pooja</v>
       </c>
       <c r="D6" t="str">
+        <v>9096648553</v>
+      </c>
+      <c r="E6" t="str">
+        <v>A 1608, Pune 411045</v>
+      </c>
+      <c r="F6" t="str">
+        <v>Girl Haldi Kunku Set x1</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6" t="str">
+        <v>NEW</v>
+      </c>
+      <c r="I6" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J6" t="str">
+        <v/>
+      </c>
+      <c r="K6" t="str">
+        <v/>
+      </c>
+      <c r="L6" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="7" xml:space="preserve">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7" t="str">
+        <v>2026-01-13 10:20</v>
+      </c>
+      <c r="C7" t="str">
+        <v>Pooja</v>
+      </c>
+      <c r="D7" t="str">
         <v>02030443000</v>
       </c>
-      <c r="E6" t="str" xml:space="preserve">
+      <c r="E7" t="str" xml:space="preserve">
         <v xml:space="preserve">Level 1, Tower S3, CyberCity,
 Magarpatta City, Hadapsar, PUNE 411013</v>
       </c>
-      <c r="F6" t="str">
+      <c r="F7" t="str">
         <v>Girl Holding Hands Thali x1</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6" t="str">
-        <v>NEW</v>
-      </c>
-      <c r="I6" t="str">
-        <v>PENDING</v>
-      </c>
-      <c r="J6" t="str">
-        <v/>
-      </c>
-      <c r="K6" t="str">
-        <v/>
-      </c>
-      <c r="L6" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7">
-        <v>1</v>
-      </c>
-      <c r="B7" t="str">
-        <v>2026-01-13 09:36</v>
-      </c>
-      <c r="C7" t="str">
-        <v>Pooja</v>
-      </c>
-      <c r="D7" t="str">
-        <v>9096648553</v>
-      </c>
-      <c r="E7" t="str">
-        <v>A 1608, Pune 411045</v>
-      </c>
-      <c r="F7" t="str">
-        <v>Girl Haldi Kunku Set x10</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -671,9 +671,47 @@
         <v/>
       </c>
     </row>
+    <row r="8">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="str">
+        <v>2026-01-13 09:36</v>
+      </c>
+      <c r="C8" t="str">
+        <v>Pooja</v>
+      </c>
+      <c r="D8" t="str">
+        <v>9096648553</v>
+      </c>
+      <c r="E8" t="str">
+        <v>A 1608, Pune 411045</v>
+      </c>
+      <c r="F8" t="str">
+        <v>Girl Haldi Kunku Set x10</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8" t="str">
+        <v>NEW</v>
+      </c>
+      <c r="I8" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J8" t="str">
+        <v/>
+      </c>
+      <c r="K8" t="str">
+        <v/>
+      </c>
+      <c r="L8" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L8"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -713,7 +751,7 @@
         <v>2026-01-13</v>
       </c>
       <c r="B2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -722,13 +760,13 @@
         <v>1</v>
       </c>
       <c r="E2">
-        <v>25</v>
+        <v>325</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>25</v>
+        <v>325</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
📊 Update UrbanGulal_Consolidated_2026-01-13.xlsx - 2026-01-13T18:56:55.251Z
</commit_message>
<xml_diff>
--- a/reports/UrbanGulal_Consolidated_2026-01-13.xlsx
+++ b/reports/UrbanGulal_Consolidated_2026-01-13.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -443,10 +443,10 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" t="str">
-        <v>2026-01-13 18:48</v>
+        <v>2026-01-13 18:56</v>
       </c>
       <c r="C2" t="str">
         <v>Sagar Borse</v>
@@ -455,16 +455,16 @@
         <v>7588930329</v>
       </c>
       <c r="E2" t="str">
-        <v>Test2,</v>
+        <v>Test3,</v>
       </c>
       <c r="F2" t="str">
-        <v>Kite Haldi Kunku Set x10</v>
+        <v>Square Heat Pad x1</v>
       </c>
       <c r="G2">
-        <v>300</v>
+        <v>50</v>
       </c>
       <c r="H2" t="str">
-        <v>CONFIRMED</v>
+        <v>NEW</v>
       </c>
       <c r="I2" t="str">
         <v>PENDING</v>
@@ -481,10 +481,10 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" t="str">
-        <v>2026-01-13 18:47</v>
+        <v>2026-01-13 18:48</v>
       </c>
       <c r="C3" t="str">
         <v>Sagar Borse</v>
@@ -493,16 +493,16 @@
         <v>7588930329</v>
       </c>
       <c r="E3" t="str">
-        <v>Test,</v>
+        <v>Test2,</v>
       </c>
       <c r="F3" t="str">
-        <v>Girl Haldi Kunku Set x1</v>
+        <v>Kite Haldi Kunku Set x10</v>
       </c>
       <c r="G3">
-        <v>25</v>
+        <v>300</v>
       </c>
       <c r="H3" t="str">
-        <v>NEW</v>
+        <v>CONFIRMED</v>
       </c>
       <c r="I3" t="str">
         <v>PENDING</v>
@@ -517,69 +517,69 @@
         <v/>
       </c>
     </row>
-    <row r="4" xml:space="preserve">
+    <row r="4">
       <c r="A4">
+        <v>6</v>
+      </c>
+      <c r="B4" t="str">
+        <v>2026-01-13 18:47</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Sagar Borse</v>
+      </c>
+      <c r="D4" t="str">
+        <v>7588930329</v>
+      </c>
+      <c r="E4" t="str">
+        <v>Test,</v>
+      </c>
+      <c r="F4" t="str">
+        <v>Girl Haldi Kunku Set x1</v>
+      </c>
+      <c r="G4">
+        <v>25</v>
+      </c>
+      <c r="H4" t="str">
+        <v>NEW</v>
+      </c>
+      <c r="I4" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J4" t="str">
+        <v/>
+      </c>
+      <c r="K4" t="str">
+        <v/>
+      </c>
+      <c r="L4" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="5" xml:space="preserve">
+      <c r="A5">
         <v>5</v>
       </c>
-      <c r="B4" t="str">
+      <c r="B5" t="str">
         <v>2026-01-13 16:54</v>
       </c>
-      <c r="C4" t="str">
+      <c r="C5" t="str">
         <v>Pooja</v>
       </c>
-      <c r="D4" t="str">
+      <c r="D5" t="str">
         <v>9096648553</v>
       </c>
-      <c r="E4" t="str" xml:space="preserve">
+      <c r="E5" t="str" xml:space="preserve">
         <v xml:space="preserve">Level 1, Tower S3, CyberCity,
 Magarpatta City, Hadapsar, PUNE 411013</v>
       </c>
-      <c r="F4" t="str">
+      <c r="F5" t="str">
         <v>Girl Holding Hands Thali x1</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4" t="str">
-        <v>NEW</v>
-      </c>
-      <c r="I4" t="str">
-        <v>PENDING</v>
-      </c>
-      <c r="J4" t="str">
-        <v/>
-      </c>
-      <c r="K4" t="str">
-        <v/>
-      </c>
-      <c r="L4" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="str">
-        <v>2026-01-13 10:51</v>
-      </c>
-      <c r="C5" t="str">
-        <v>Ajay Dwarkunde</v>
-      </c>
-      <c r="D5" t="str">
-        <v>8087172173</v>
-      </c>
-      <c r="E5" t="str">
-        <v>wakad, pune 411057</v>
-      </c>
-      <c r="F5" t="str">
-        <v>Girl Holding Hands Thali x1, Kalash Haldi Kunku (Golden) x1, Kite Haldi Kunku Set x1</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
       <c r="H5" t="str">
-        <v>CANCELLED</v>
+        <v>NEW</v>
       </c>
       <c r="I5" t="str">
         <v>PENDING</v>
@@ -588,7 +588,7 @@
         <v/>
       </c>
       <c r="K5" t="str">
-        <v>test</v>
+        <v/>
       </c>
       <c r="L5" t="str">
         <v/>
@@ -596,28 +596,28 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6" t="str">
-        <v>2026-01-13 10:38</v>
+        <v>2026-01-13 10:51</v>
       </c>
       <c r="C6" t="str">
-        <v>Pooja</v>
+        <v>Ajay Dwarkunde</v>
       </c>
       <c r="D6" t="str">
-        <v>9096648553</v>
+        <v>8087172173</v>
       </c>
       <c r="E6" t="str">
-        <v>A 1608, Pune 411045</v>
+        <v>wakad, pune 411057</v>
       </c>
       <c r="F6" t="str">
-        <v>Girl Haldi Kunku Set x1</v>
+        <v>Girl Holding Hands Thali x1, Kalash Haldi Kunku (Golden) x1, Kite Haldi Kunku Set x1</v>
       </c>
       <c r="G6">
         <v>0</v>
       </c>
       <c r="H6" t="str">
-        <v>NEW</v>
+        <v>CANCELLED</v>
       </c>
       <c r="I6" t="str">
         <v>PENDING</v>
@@ -626,69 +626,69 @@
         <v/>
       </c>
       <c r="K6" t="str">
-        <v/>
+        <v>test</v>
       </c>
       <c r="L6" t="str">
         <v/>
       </c>
     </row>
-    <row r="7" xml:space="preserve">
+    <row r="7">
       <c r="A7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B7" t="str">
-        <v>2026-01-13 10:20</v>
+        <v>2026-01-13 10:38</v>
       </c>
       <c r="C7" t="str">
         <v>Pooja</v>
       </c>
       <c r="D7" t="str">
+        <v>9096648553</v>
+      </c>
+      <c r="E7" t="str">
+        <v>A 1608, Pune 411045</v>
+      </c>
+      <c r="F7" t="str">
+        <v>Girl Haldi Kunku Set x1</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7" t="str">
+        <v>NEW</v>
+      </c>
+      <c r="I7" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J7" t="str">
+        <v/>
+      </c>
+      <c r="K7" t="str">
+        <v/>
+      </c>
+      <c r="L7" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="8" xml:space="preserve">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8" t="str">
+        <v>2026-01-13 10:20</v>
+      </c>
+      <c r="C8" t="str">
+        <v>Pooja</v>
+      </c>
+      <c r="D8" t="str">
         <v>02030443000</v>
       </c>
-      <c r="E7" t="str" xml:space="preserve">
+      <c r="E8" t="str" xml:space="preserve">
         <v xml:space="preserve">Level 1, Tower S3, CyberCity,
 Magarpatta City, Hadapsar, PUNE 411013</v>
       </c>
-      <c r="F7" t="str">
+      <c r="F8" t="str">
         <v>Girl Holding Hands Thali x1</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7" t="str">
-        <v>NEW</v>
-      </c>
-      <c r="I7" t="str">
-        <v>PENDING</v>
-      </c>
-      <c r="J7" t="str">
-        <v/>
-      </c>
-      <c r="K7" t="str">
-        <v/>
-      </c>
-      <c r="L7" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8" t="str">
-        <v>2026-01-13 09:36</v>
-      </c>
-      <c r="C8" t="str">
-        <v>Pooja</v>
-      </c>
-      <c r="D8" t="str">
-        <v>9096648553</v>
-      </c>
-      <c r="E8" t="str">
-        <v>A 1608, Pune 411045</v>
-      </c>
-      <c r="F8" t="str">
-        <v>Girl Haldi Kunku Set x10</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -709,9 +709,47 @@
         <v/>
       </c>
     </row>
+    <row r="9">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" t="str">
+        <v>2026-01-13 09:36</v>
+      </c>
+      <c r="C9" t="str">
+        <v>Pooja</v>
+      </c>
+      <c r="D9" t="str">
+        <v>9096648553</v>
+      </c>
+      <c r="E9" t="str">
+        <v>A 1608, Pune 411045</v>
+      </c>
+      <c r="F9" t="str">
+        <v>Girl Haldi Kunku Set x10</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9" t="str">
+        <v>NEW</v>
+      </c>
+      <c r="I9" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J9" t="str">
+        <v/>
+      </c>
+      <c r="K9" t="str">
+        <v/>
+      </c>
+      <c r="L9" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L9"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -751,7 +789,7 @@
         <v>2026-01-13</v>
       </c>
       <c r="B2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -760,13 +798,13 @@
         <v>1</v>
       </c>
       <c r="E2">
-        <v>325</v>
+        <v>375</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>325</v>
+        <v>375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
📊 Update UrbanGulal_Consolidated_2026-01-13.xlsx - 2026-01-13T19:05:58.350Z
</commit_message>
<xml_diff>
--- a/reports/UrbanGulal_Consolidated_2026-01-13.xlsx
+++ b/reports/UrbanGulal_Consolidated_2026-01-13.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -443,10 +443,10 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" t="str">
-        <v>2026-01-13 18:56</v>
+        <v>2026-01-13 19:05</v>
       </c>
       <c r="C2" t="str">
         <v>Sagar Borse</v>
@@ -455,16 +455,16 @@
         <v>7588930329</v>
       </c>
       <c r="E2" t="str">
-        <v>Test3,</v>
+        <v>Test,</v>
       </c>
       <c r="F2" t="str">
-        <v>Square Heat Pad x1</v>
+        <v>Stainless Steel Grater x1, Square Heat Pad x1, Circle Heat Pad x1, Leaf Tray (Large) x1</v>
       </c>
       <c r="G2">
-        <v>50</v>
+        <v>185</v>
       </c>
       <c r="H2" t="str">
-        <v>CONFIRMED</v>
+        <v>NEW</v>
       </c>
       <c r="I2" t="str">
         <v>PENDING</v>
@@ -481,10 +481,10 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" t="str">
-        <v>2026-01-13 18:48</v>
+        <v>2026-01-13 18:56</v>
       </c>
       <c r="C3" t="str">
         <v>Sagar Borse</v>
@@ -493,13 +493,13 @@
         <v>7588930329</v>
       </c>
       <c r="E3" t="str">
-        <v>Test2,</v>
+        <v>Test3,</v>
       </c>
       <c r="F3" t="str">
-        <v>Kite Haldi Kunku Set x10</v>
+        <v>Square Heat Pad x1</v>
       </c>
       <c r="G3">
-        <v>300</v>
+        <v>50</v>
       </c>
       <c r="H3" t="str">
         <v>CONFIRMED</v>
@@ -519,10 +519,10 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" t="str">
-        <v>2026-01-13 18:47</v>
+        <v>2026-01-13 18:48</v>
       </c>
       <c r="C4" t="str">
         <v>Sagar Borse</v>
@@ -531,16 +531,16 @@
         <v>7588930329</v>
       </c>
       <c r="E4" t="str">
-        <v>Test,</v>
+        <v>Test2,</v>
       </c>
       <c r="F4" t="str">
-        <v>Girl Haldi Kunku Set x1</v>
+        <v>Kite Haldi Kunku Set x10</v>
       </c>
       <c r="G4">
-        <v>25</v>
+        <v>300</v>
       </c>
       <c r="H4" t="str">
-        <v>NEW</v>
+        <v>CONFIRMED</v>
       </c>
       <c r="I4" t="str">
         <v>PENDING</v>
@@ -555,69 +555,69 @@
         <v/>
       </c>
     </row>
-    <row r="5" xml:space="preserve">
+    <row r="5">
       <c r="A5">
+        <v>6</v>
+      </c>
+      <c r="B5" t="str">
+        <v>2026-01-13 18:47</v>
+      </c>
+      <c r="C5" t="str">
+        <v>Sagar Borse</v>
+      </c>
+      <c r="D5" t="str">
+        <v>7588930329</v>
+      </c>
+      <c r="E5" t="str">
+        <v>Test,</v>
+      </c>
+      <c r="F5" t="str">
+        <v>Girl Haldi Kunku Set x1</v>
+      </c>
+      <c r="G5">
+        <v>25</v>
+      </c>
+      <c r="H5" t="str">
+        <v>NEW</v>
+      </c>
+      <c r="I5" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J5" t="str">
+        <v/>
+      </c>
+      <c r="K5" t="str">
+        <v/>
+      </c>
+      <c r="L5" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="6" xml:space="preserve">
+      <c r="A6">
         <v>5</v>
       </c>
-      <c r="B5" t="str">
+      <c r="B6" t="str">
         <v>2026-01-13 16:54</v>
       </c>
-      <c r="C5" t="str">
+      <c r="C6" t="str">
         <v>Pooja</v>
       </c>
-      <c r="D5" t="str">
+      <c r="D6" t="str">
         <v>9096648553</v>
       </c>
-      <c r="E5" t="str" xml:space="preserve">
+      <c r="E6" t="str" xml:space="preserve">
         <v xml:space="preserve">Level 1, Tower S3, CyberCity,
 Magarpatta City, Hadapsar, PUNE 411013</v>
       </c>
-      <c r="F5" t="str">
+      <c r="F6" t="str">
         <v>Girl Holding Hands Thali x1</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5" t="str">
-        <v>NEW</v>
-      </c>
-      <c r="I5" t="str">
-        <v>PENDING</v>
-      </c>
-      <c r="J5" t="str">
-        <v/>
-      </c>
-      <c r="K5" t="str">
-        <v/>
-      </c>
-      <c r="L5" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" t="str">
-        <v>2026-01-13 10:51</v>
-      </c>
-      <c r="C6" t="str">
-        <v>Ajay Dwarkunde</v>
-      </c>
-      <c r="D6" t="str">
-        <v>8087172173</v>
-      </c>
-      <c r="E6" t="str">
-        <v>wakad, pune 411057</v>
-      </c>
-      <c r="F6" t="str">
-        <v>Girl Holding Hands Thali x1, Kalash Haldi Kunku (Golden) x1, Kite Haldi Kunku Set x1</v>
       </c>
       <c r="G6">
         <v>0</v>
       </c>
       <c r="H6" t="str">
-        <v>CANCELLED</v>
+        <v>NEW</v>
       </c>
       <c r="I6" t="str">
         <v>PENDING</v>
@@ -626,7 +626,7 @@
         <v/>
       </c>
       <c r="K6" t="str">
-        <v>test</v>
+        <v/>
       </c>
       <c r="L6" t="str">
         <v/>
@@ -634,28 +634,28 @@
     </row>
     <row r="7">
       <c r="A7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B7" t="str">
-        <v>2026-01-13 10:38</v>
+        <v>2026-01-13 10:51</v>
       </c>
       <c r="C7" t="str">
-        <v>Pooja</v>
+        <v>Ajay Dwarkunde</v>
       </c>
       <c r="D7" t="str">
-        <v>9096648553</v>
+        <v>8087172173</v>
       </c>
       <c r="E7" t="str">
-        <v>A 1608, Pune 411045</v>
+        <v>wakad, pune 411057</v>
       </c>
       <c r="F7" t="str">
-        <v>Girl Haldi Kunku Set x1</v>
+        <v>Girl Holding Hands Thali x1, Kalash Haldi Kunku (Golden) x1, Kite Haldi Kunku Set x1</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7" t="str">
-        <v>NEW</v>
+        <v>CANCELLED</v>
       </c>
       <c r="I7" t="str">
         <v>PENDING</v>
@@ -664,69 +664,69 @@
         <v/>
       </c>
       <c r="K7" t="str">
-        <v/>
+        <v>test</v>
       </c>
       <c r="L7" t="str">
         <v/>
       </c>
     </row>
-    <row r="8" xml:space="preserve">
+    <row r="8">
       <c r="A8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B8" t="str">
-        <v>2026-01-13 10:20</v>
+        <v>2026-01-13 10:38</v>
       </c>
       <c r="C8" t="str">
         <v>Pooja</v>
       </c>
       <c r="D8" t="str">
+        <v>9096648553</v>
+      </c>
+      <c r="E8" t="str">
+        <v>A 1608, Pune 411045</v>
+      </c>
+      <c r="F8" t="str">
+        <v>Girl Haldi Kunku Set x1</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8" t="str">
+        <v>NEW</v>
+      </c>
+      <c r="I8" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J8" t="str">
+        <v/>
+      </c>
+      <c r="K8" t="str">
+        <v/>
+      </c>
+      <c r="L8" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="9" xml:space="preserve">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9" t="str">
+        <v>2026-01-13 10:20</v>
+      </c>
+      <c r="C9" t="str">
+        <v>Pooja</v>
+      </c>
+      <c r="D9" t="str">
         <v>02030443000</v>
       </c>
-      <c r="E8" t="str" xml:space="preserve">
+      <c r="E9" t="str" xml:space="preserve">
         <v xml:space="preserve">Level 1, Tower S3, CyberCity,
 Magarpatta City, Hadapsar, PUNE 411013</v>
       </c>
-      <c r="F8" t="str">
+      <c r="F9" t="str">
         <v>Girl Holding Hands Thali x1</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8" t="str">
-        <v>NEW</v>
-      </c>
-      <c r="I8" t="str">
-        <v>PENDING</v>
-      </c>
-      <c r="J8" t="str">
-        <v/>
-      </c>
-      <c r="K8" t="str">
-        <v/>
-      </c>
-      <c r="L8" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9">
-        <v>1</v>
-      </c>
-      <c r="B9" t="str">
-        <v>2026-01-13 09:36</v>
-      </c>
-      <c r="C9" t="str">
-        <v>Pooja</v>
-      </c>
-      <c r="D9" t="str">
-        <v>9096648553</v>
-      </c>
-      <c r="E9" t="str">
-        <v>A 1608, Pune 411045</v>
-      </c>
-      <c r="F9" t="str">
-        <v>Girl Haldi Kunku Set x10</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -747,9 +747,47 @@
         <v/>
       </c>
     </row>
+    <row r="10">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="str">
+        <v>2026-01-13 09:36</v>
+      </c>
+      <c r="C10" t="str">
+        <v>Pooja</v>
+      </c>
+      <c r="D10" t="str">
+        <v>9096648553</v>
+      </c>
+      <c r="E10" t="str">
+        <v>A 1608, Pune 411045</v>
+      </c>
+      <c r="F10" t="str">
+        <v>Girl Haldi Kunku Set x10</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10" t="str">
+        <v>NEW</v>
+      </c>
+      <c r="I10" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J10" t="str">
+        <v/>
+      </c>
+      <c r="K10" t="str">
+        <v/>
+      </c>
+      <c r="L10" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L9"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L10"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -789,7 +827,7 @@
         <v>2026-01-13</v>
       </c>
       <c r="B2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -798,13 +836,13 @@
         <v>1</v>
       </c>
       <c r="E2">
-        <v>375</v>
+        <v>560</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>375</v>
+        <v>560</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
📊 Update UrbanGulal_Consolidated_2026-01-13.xlsx - 2026-01-13T19:11:51.701Z
</commit_message>
<xml_diff>
--- a/reports/UrbanGulal_Consolidated_2026-01-13.xlsx
+++ b/reports/UrbanGulal_Consolidated_2026-01-13.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -443,10 +443,10 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" t="str">
-        <v>2026-01-13 19:05</v>
+        <v>2026-01-13 19:11</v>
       </c>
       <c r="C2" t="str">
         <v>Sagar Borse</v>
@@ -458,10 +458,10 @@
         <v>Test,</v>
       </c>
       <c r="F2" t="str">
-        <v>Stainless Steel Grater x1, Square Heat Pad x1, Circle Heat Pad x1, Leaf Tray (Large) x1</v>
+        <v>Stainless Steel Grater x1</v>
       </c>
       <c r="G2">
-        <v>185</v>
+        <v>40</v>
       </c>
       <c r="H2" t="str">
         <v>NEW</v>
@@ -481,10 +481,10 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" t="str">
-        <v>2026-01-13 18:56</v>
+        <v>2026-01-13 19:05</v>
       </c>
       <c r="C3" t="str">
         <v>Sagar Borse</v>
@@ -493,16 +493,16 @@
         <v>7588930329</v>
       </c>
       <c r="E3" t="str">
-        <v>Test3,</v>
+        <v>Test,</v>
       </c>
       <c r="F3" t="str">
-        <v>Square Heat Pad x1</v>
+        <v>Stainless Steel Grater x1, Square Heat Pad x1, Circle Heat Pad x1, Leaf Tray (Large) x1</v>
       </c>
       <c r="G3">
-        <v>50</v>
+        <v>185</v>
       </c>
       <c r="H3" t="str">
-        <v>CONFIRMED</v>
+        <v>NEW</v>
       </c>
       <c r="I3" t="str">
         <v>PENDING</v>
@@ -519,10 +519,10 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" t="str">
-        <v>2026-01-13 18:48</v>
+        <v>2026-01-13 18:56</v>
       </c>
       <c r="C4" t="str">
         <v>Sagar Borse</v>
@@ -531,13 +531,13 @@
         <v>7588930329</v>
       </c>
       <c r="E4" t="str">
-        <v>Test2,</v>
+        <v>Test3,</v>
       </c>
       <c r="F4" t="str">
-        <v>Kite Haldi Kunku Set x10</v>
+        <v>Square Heat Pad x1</v>
       </c>
       <c r="G4">
-        <v>300</v>
+        <v>50</v>
       </c>
       <c r="H4" t="str">
         <v>CONFIRMED</v>
@@ -557,10 +557,10 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" t="str">
-        <v>2026-01-13 18:47</v>
+        <v>2026-01-13 18:48</v>
       </c>
       <c r="C5" t="str">
         <v>Sagar Borse</v>
@@ -569,93 +569,93 @@
         <v>7588930329</v>
       </c>
       <c r="E5" t="str">
+        <v>Test2,</v>
+      </c>
+      <c r="F5" t="str">
+        <v>Kite Haldi Kunku Set x10</v>
+      </c>
+      <c r="G5">
+        <v>300</v>
+      </c>
+      <c r="H5" t="str">
+        <v>CONFIRMED</v>
+      </c>
+      <c r="I5" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J5" t="str">
+        <v/>
+      </c>
+      <c r="K5" t="str">
+        <v/>
+      </c>
+      <c r="L5" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" t="str">
+        <v>2026-01-13 18:47</v>
+      </c>
+      <c r="C6" t="str">
+        <v>Sagar Borse</v>
+      </c>
+      <c r="D6" t="str">
+        <v>7588930329</v>
+      </c>
+      <c r="E6" t="str">
         <v>Test,</v>
       </c>
-      <c r="F5" t="str">
+      <c r="F6" t="str">
         <v>Girl Haldi Kunku Set x1</v>
       </c>
-      <c r="G5">
+      <c r="G6">
         <v>25</v>
       </c>
-      <c r="H5" t="str">
+      <c r="H6" t="str">
         <v>NEW</v>
       </c>
-      <c r="I5" t="str">
-        <v>PENDING</v>
-      </c>
-      <c r="J5" t="str">
-        <v/>
-      </c>
-      <c r="K5" t="str">
-        <v/>
-      </c>
-      <c r="L5" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="6" xml:space="preserve">
-      <c r="A6">
+      <c r="I6" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J6" t="str">
+        <v/>
+      </c>
+      <c r="K6" t="str">
+        <v/>
+      </c>
+      <c r="L6" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="7" xml:space="preserve">
+      <c r="A7">
         <v>5</v>
       </c>
-      <c r="B6" t="str">
+      <c r="B7" t="str">
         <v>2026-01-13 16:54</v>
       </c>
-      <c r="C6" t="str">
+      <c r="C7" t="str">
         <v>Pooja</v>
       </c>
-      <c r="D6" t="str">
+      <c r="D7" t="str">
         <v>9096648553</v>
       </c>
-      <c r="E6" t="str" xml:space="preserve">
+      <c r="E7" t="str" xml:space="preserve">
         <v xml:space="preserve">Level 1, Tower S3, CyberCity,
 Magarpatta City, Hadapsar, PUNE 411013</v>
       </c>
-      <c r="F6" t="str">
+      <c r="F7" t="str">
         <v>Girl Holding Hands Thali x1</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6" t="str">
-        <v>NEW</v>
-      </c>
-      <c r="I6" t="str">
-        <v>PENDING</v>
-      </c>
-      <c r="J6" t="str">
-        <v/>
-      </c>
-      <c r="K6" t="str">
-        <v/>
-      </c>
-      <c r="L6" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7">
-        <v>4</v>
-      </c>
-      <c r="B7" t="str">
-        <v>2026-01-13 10:51</v>
-      </c>
-      <c r="C7" t="str">
-        <v>Ajay Dwarkunde</v>
-      </c>
-      <c r="D7" t="str">
-        <v>8087172173</v>
-      </c>
-      <c r="E7" t="str">
-        <v>wakad, pune 411057</v>
-      </c>
-      <c r="F7" t="str">
-        <v>Girl Holding Hands Thali x1, Kalash Haldi Kunku (Golden) x1, Kite Haldi Kunku Set x1</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7" t="str">
-        <v>CANCELLED</v>
+        <v>NEW</v>
       </c>
       <c r="I7" t="str">
         <v>PENDING</v>
@@ -664,7 +664,7 @@
         <v/>
       </c>
       <c r="K7" t="str">
-        <v>test</v>
+        <v/>
       </c>
       <c r="L7" t="str">
         <v/>
@@ -672,28 +672,28 @@
     </row>
     <row r="8">
       <c r="A8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B8" t="str">
-        <v>2026-01-13 10:38</v>
+        <v>2026-01-13 10:51</v>
       </c>
       <c r="C8" t="str">
-        <v>Pooja</v>
+        <v>Ajay Dwarkunde</v>
       </c>
       <c r="D8" t="str">
-        <v>9096648553</v>
+        <v>8087172173</v>
       </c>
       <c r="E8" t="str">
-        <v>A 1608, Pune 411045</v>
+        <v>wakad, pune 411057</v>
       </c>
       <c r="F8" t="str">
-        <v>Girl Haldi Kunku Set x1</v>
+        <v>Girl Holding Hands Thali x1, Kalash Haldi Kunku (Golden) x1, Kite Haldi Kunku Set x1</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
       <c r="H8" t="str">
-        <v>NEW</v>
+        <v>CANCELLED</v>
       </c>
       <c r="I8" t="str">
         <v>PENDING</v>
@@ -702,69 +702,69 @@
         <v/>
       </c>
       <c r="K8" t="str">
-        <v/>
+        <v>test</v>
       </c>
       <c r="L8" t="str">
         <v/>
       </c>
     </row>
-    <row r="9" xml:space="preserve">
+    <row r="9">
       <c r="A9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B9" t="str">
-        <v>2026-01-13 10:20</v>
+        <v>2026-01-13 10:38</v>
       </c>
       <c r="C9" t="str">
         <v>Pooja</v>
       </c>
       <c r="D9" t="str">
+        <v>9096648553</v>
+      </c>
+      <c r="E9" t="str">
+        <v>A 1608, Pune 411045</v>
+      </c>
+      <c r="F9" t="str">
+        <v>Girl Haldi Kunku Set x1</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9" t="str">
+        <v>NEW</v>
+      </c>
+      <c r="I9" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J9" t="str">
+        <v/>
+      </c>
+      <c r="K9" t="str">
+        <v/>
+      </c>
+      <c r="L9" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="10" xml:space="preserve">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10" t="str">
+        <v>2026-01-13 10:20</v>
+      </c>
+      <c r="C10" t="str">
+        <v>Pooja</v>
+      </c>
+      <c r="D10" t="str">
         <v>02030443000</v>
       </c>
-      <c r="E9" t="str" xml:space="preserve">
+      <c r="E10" t="str" xml:space="preserve">
         <v xml:space="preserve">Level 1, Tower S3, CyberCity,
 Magarpatta City, Hadapsar, PUNE 411013</v>
       </c>
-      <c r="F9" t="str">
+      <c r="F10" t="str">
         <v>Girl Holding Hands Thali x1</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9" t="str">
-        <v>NEW</v>
-      </c>
-      <c r="I9" t="str">
-        <v>PENDING</v>
-      </c>
-      <c r="J9" t="str">
-        <v/>
-      </c>
-      <c r="K9" t="str">
-        <v/>
-      </c>
-      <c r="L9" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10">
-        <v>1</v>
-      </c>
-      <c r="B10" t="str">
-        <v>2026-01-13 09:36</v>
-      </c>
-      <c r="C10" t="str">
-        <v>Pooja</v>
-      </c>
-      <c r="D10" t="str">
-        <v>9096648553</v>
-      </c>
-      <c r="E10" t="str">
-        <v>A 1608, Pune 411045</v>
-      </c>
-      <c r="F10" t="str">
-        <v>Girl Haldi Kunku Set x10</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -785,9 +785,47 @@
         <v/>
       </c>
     </row>
+    <row r="11">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="str">
+        <v>2026-01-13 09:36</v>
+      </c>
+      <c r="C11" t="str">
+        <v>Pooja</v>
+      </c>
+      <c r="D11" t="str">
+        <v>9096648553</v>
+      </c>
+      <c r="E11" t="str">
+        <v>A 1608, Pune 411045</v>
+      </c>
+      <c r="F11" t="str">
+        <v>Girl Haldi Kunku Set x10</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11" t="str">
+        <v>NEW</v>
+      </c>
+      <c r="I11" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J11" t="str">
+        <v/>
+      </c>
+      <c r="K11" t="str">
+        <v/>
+      </c>
+      <c r="L11" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L10"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L11"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -827,7 +865,7 @@
         <v>2026-01-13</v>
       </c>
       <c r="B2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -836,13 +874,13 @@
         <v>1</v>
       </c>
       <c r="E2">
-        <v>560</v>
+        <v>600</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>560</v>
+        <v>600</v>
       </c>
     </row>
   </sheetData>

</xml_diff>